<commit_message>
Created save_object function to improve output file storage
Small improvements to the PE Markdown and significant progress on protein analysis.
</commit_message>
<xml_diff>
--- a/protein/input_prot/calibration_prot.xlsx
+++ b/protein/input_prot/calibration_prot.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\trevo\OneDrive\Documents\GitHub\TEdissy_analysis\protein\input_prot\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\23012218\Desktop\TEdissy_analysis\protein\input_prot\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A2649181-6919-4ADA-BD25-1B1EC2FF3E9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1F01B5C2-4406-409C-BA7A-7D047284364D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="20" yWindow="620" windowWidth="19180" windowHeight="10180" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="24240" windowHeight="17520" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -365,15 +365,15 @@
   <dimension ref="A1:C13"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B3" sqref="B3"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="15.7265625" customWidth="1"/>
+    <col min="1" max="1" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -384,7 +384,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>0</v>
       </c>
@@ -395,7 +395,7 @@
         <v>2.4999999999999953E-3</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -406,7 +406,7 @@
         <v>-2.5000000000000022E-3</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1.2</v>
       </c>
@@ -417,7 +417,7 @@
         <v>0.25850000000000001</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2.4</v>
       </c>
@@ -428,7 +428,7 @@
         <v>0.32350000000000001</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -439,7 +439,7 @@
         <v>0.44550000000000001</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>3.6</v>
       </c>
@@ -450,7 +450,7 @@
         <v>0.5575</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>4.8</v>
       </c>
@@ -461,7 +461,7 @@
         <v>0.77849999999999997</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1.2</v>
       </c>
@@ -472,29 +472,29 @@
         <v>0.18083333330000001</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>2.4</v>
       </c>
       <c r="B10">
-        <v>0.32350000000000001</v>
+        <v>0.505</v>
       </c>
       <c r="C10">
-        <v>0.27300000000000002</v>
-      </c>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+        <v>0.45450000000000002</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>3</v>
       </c>
       <c r="B11">
-        <v>0.44550000000000001</v>
+        <v>0.55500000000000005</v>
       </c>
       <c r="C11">
-        <v>0.39500000000000002</v>
-      </c>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+        <v>0.50450000000000006</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>3.6</v>
       </c>
@@ -505,7 +505,7 @@
         <v>0.58483333329999998</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>4.8</v>
       </c>

</xml_diff>